<commit_message>
update tableau acquisition Nathan
</commit_message>
<xml_diff>
--- a/Acquisition_mouvement_Kev_Nath_11.11.xlsx
+++ b/Acquisition_mouvement_Kev_Nath_11.11.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\Avat-Art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA314715-36C5-4F37-9C80-12E10788C90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874EAAFC-09D0-4D04-ACEA-B684AD7D281F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition" sheetId="1" r:id="rId1"/>
     <sheet name="Analyse" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Acquisition!$A$2:$AE$303</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Acquisition!$A$2:$AE$304</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="42">
   <si>
     <t>Acqusition</t>
   </si>
@@ -148,6 +148,9 @@
   <si>
     <t>La distance entre 2 jointures (main droite et coude droite) est différente selon la distance entre le cobbaye et la Kinect. Donc, pour les critères de détection de mouvement, il faut bien comparer des joints entre eux et garder leur proportionalité plutôt que leur demander de dépasser un certain seuil qui serait différent selon la dsitance à la Kinect</t>
   </si>
+  <si>
+    <t>Taille tête</t>
+  </si>
 </sst>
 </file>
 
@@ -236,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +277,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -552,6 +561,9 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -564,8 +576,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="4" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -875,9 +887,9 @@
   </sheetPr>
   <dimension ref="A1:XET377"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG16" sqref="AG16"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB127" sqref="AB127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -895,11 +907,11 @@
     <col min="31" max="31" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:34" ht="34.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -908,10 +920,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="50" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -989,10 +1001,13 @@
       <c r="AE1" s="2">
         <v>3</v>
       </c>
+      <c r="AF1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="48"/>
+    <row r="2" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="47"/>
+      <c r="B2" s="49"/>
       <c r="C2" s="3">
         <v>1</v>
       </c>
@@ -22354,7 +22369,7 @@
         <v>0.32128819823265081</v>
       </c>
     </row>
-    <row r="241" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="13">
         <f t="shared" si="3"/>
         <v>80</v>
@@ -22453,8 +22468,12 @@
         <f>AC241/((L241+W241)/2)</f>
         <v>0.21474035011026701</v>
       </c>
+      <c r="AF241" s="24">
+        <f>ABS(F241-E241)</f>
+        <v>0.16423529386520386</v>
+      </c>
     </row>
-    <row r="242" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="16">
         <f t="shared" si="3"/>
         <v>80</v>
@@ -22538,7 +22557,7 @@
         <v>2.5154285430908199</v>
       </c>
     </row>
-    <row r="243" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="6">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -22622,7 +22641,7 @@
         <v>0.17331609129905701</v>
       </c>
     </row>
-    <row r="244" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="6">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -22721,8 +22740,12 @@
         <f>AC244/((L244+W244)/2)</f>
         <v>0.17496022879356948</v>
       </c>
+      <c r="AF244" s="24">
+        <f>ABS(F244-E244)</f>
+        <v>0.16659048199653631</v>
+      </c>
     </row>
-    <row r="245" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="6">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -22806,7 +22829,7 @@
         <v>2.6849524974822998</v>
       </c>
     </row>
-    <row r="246" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="10">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -22890,7 +22913,7 @@
         <v>0.45863226056098938</v>
       </c>
     </row>
-    <row r="247" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="13">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -22989,8 +23012,12 @@
         <f>AC247/((L247+W247)/2)</f>
         <v>8.2123819545415491E-2</v>
       </c>
+      <c r="AF247" s="24">
+        <f>ABS(F247-E247)</f>
+        <v>0.16130870580673212</v>
+      </c>
     </row>
-    <row r="248" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="16">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -23074,7 +23101,7 @@
         <v>2.6782186031341548</v>
       </c>
     </row>
-    <row r="249" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="6">
         <f t="shared" si="3"/>
         <v>83</v>
@@ -23158,7 +23185,7 @@
         <v>0.35716056823730469</v>
       </c>
     </row>
-    <row r="250" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="6">
         <f t="shared" si="3"/>
         <v>83</v>
@@ -23257,8 +23284,12 @@
         <f>AC250/((L250+W250)/2)</f>
         <v>7.6030405358798406E-3</v>
       </c>
+      <c r="AF250" s="24">
+        <f>ABS(F250-E250)</f>
+        <v>0.15756863355636597</v>
+      </c>
     </row>
-    <row r="251" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="6">
         <f t="shared" si="3"/>
         <v>83</v>
@@ -23342,7 +23373,7 @@
         <v>2.5845000743865971</v>
       </c>
     </row>
-    <row r="252" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="10">
         <f t="shared" si="3"/>
         <v>84</v>
@@ -23426,7 +23457,7 @@
         <v>0.4078826904296875</v>
       </c>
     </row>
-    <row r="253" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="13">
         <f t="shared" si="3"/>
         <v>84</v>
@@ -23525,8 +23556,12 @@
         <f>AC253/((L253+W253)/2)</f>
         <v>-9.024221468453561E-2</v>
       </c>
+      <c r="AF253" s="24">
+        <f>ABS(F253-E253)</f>
+        <v>0.1064196825027465</v>
+      </c>
     </row>
-    <row r="254" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="16">
         <f t="shared" si="3"/>
         <v>84</v>
@@ -23610,7 +23645,7 @@
         <v>2.4054000377655029</v>
       </c>
     </row>
-    <row r="255" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="6">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -23694,7 +23729,7 @@
         <v>9.9922798573970795E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="6">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -23793,8 +23828,12 @@
         <f>AC256/((L256+W256)/2)</f>
         <v>0.41286801949654239</v>
       </c>
+      <c r="AF256" s="24">
+        <f>ABS(F256-E256)</f>
+        <v>0.14749115705490112</v>
+      </c>
     </row>
-    <row r="257" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="6">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -23878,7 +23917,7 @@
         <v>2.5663869380950932</v>
       </c>
     </row>
-    <row r="258" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="10">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -23962,7 +24001,7 @@
         <v>0.57953155040740967</v>
       </c>
     </row>
-    <row r="259" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="13">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -24061,8 +24100,12 @@
         <f>AC259/((L259+W259)/2)</f>
         <v>5.6010007520521272E-2</v>
       </c>
+      <c r="AF259" s="24">
+        <f>ABS(F259-E259)</f>
+        <v>0.14180052280426025</v>
+      </c>
     </row>
-    <row r="260" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="16">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -24146,7 +24189,7 @@
         <v>2.5991249084472661</v>
       </c>
     </row>
-    <row r="261" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="6">
         <f t="shared" si="3"/>
         <v>87</v>
@@ -24230,7 +24273,7 @@
         <v>0.24099372327327731</v>
       </c>
     </row>
-    <row r="262" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="6">
         <f t="shared" ref="A262:A302" si="4">A259+1</f>
         <v>87</v>
@@ -24329,8 +24372,12 @@
         <f>AC262/((L262+W262)/2)</f>
         <v>2.8712185143052932E-2</v>
       </c>
+      <c r="AF262" s="24">
+        <f>ABS(F262-E262)</f>
+        <v>0.14827406406402588</v>
+      </c>
     </row>
-    <row r="263" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="6">
         <f t="shared" si="4"/>
         <v>87</v>
@@ -24414,7 +24461,7 @@
         <v>2.649558544158936</v>
       </c>
     </row>
-    <row r="264" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="10">
         <f t="shared" si="4"/>
         <v>88</v>
@@ -24498,7 +24545,7 @@
         <v>0.57209765911102295</v>
       </c>
     </row>
-    <row r="265" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="13">
         <f t="shared" si="4"/>
         <v>88</v>
@@ -24597,8 +24644,12 @@
         <f>AC265/((L265+W265)/2)</f>
         <v>0.11489017399703789</v>
       </c>
+      <c r="AF265" s="24">
+        <f>ABS(F265-E265)</f>
+        <v>0.16393214464187622</v>
+      </c>
     </row>
-    <row r="266" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="16">
         <f t="shared" si="4"/>
         <v>88</v>
@@ -24682,7 +24733,7 @@
         <v>2.553777933120728</v>
       </c>
     </row>
-    <row r="267" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="6">
         <f t="shared" si="4"/>
         <v>89</v>
@@ -24766,7 +24817,7 @@
         <v>0.32114186882972717</v>
       </c>
     </row>
-    <row r="268" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="39">
         <f t="shared" si="4"/>
         <v>89</v>
@@ -24865,8 +24916,12 @@
         <f>AC268/((L268+W268)/2)</f>
         <v>0.3648311299328254</v>
       </c>
+      <c r="AF268" s="24">
+        <f>ABS(F268-E268)</f>
+        <v>0.13572984933853149</v>
+      </c>
     </row>
-    <row r="269" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="6">
         <f t="shared" si="4"/>
         <v>89</v>
@@ -24950,7 +25005,7 @@
         <v>2.6040480136871338</v>
       </c>
     </row>
-    <row r="270" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="10">
         <f t="shared" si="4"/>
         <v>90</v>
@@ -25034,7 +25089,7 @@
         <v>0.41848701238632202</v>
       </c>
     </row>
-    <row r="271" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="13">
         <f t="shared" si="4"/>
         <v>90</v>
@@ -25133,8 +25188,12 @@
         <f>AC271/((L271+W271)/2)</f>
         <v>4.0845922817670757E-2</v>
       </c>
+      <c r="AF271" s="24">
+        <f>ABS(F271-E271)</f>
+        <v>0.1364322304725647</v>
+      </c>
     </row>
-    <row r="272" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="16">
         <f t="shared" si="4"/>
         <v>90</v>
@@ -25401,7 +25460,10 @@
         <f>AC274/((L274+W274)/2)</f>
         <v>0.10720232375885609</v>
       </c>
-      <c r="AF274"/>
+      <c r="AF274" s="24">
+        <f>ABS(F274-E274)</f>
+        <v>0.15204739570617676</v>
+      </c>
       <c r="AG274"/>
       <c r="AH274"/>
       <c r="AI274"/>
@@ -42012,7 +42074,10 @@
         <f>AC277/((L277+W277)/2)</f>
         <v>5.4011172349586772E-2</v>
       </c>
-      <c r="AF277"/>
+      <c r="AF277" s="24">
+        <f>ABS(F277-E277)</f>
+        <v>0.1635054349899292</v>
+      </c>
       <c r="AG277"/>
       <c r="AH277"/>
       <c r="AI277"/>
@@ -58623,6 +58688,10 @@
         <f>AC280/((L280+W280)/2)</f>
         <v>0.12181346024917779</v>
       </c>
+      <c r="AF280" s="24">
+        <f>ABS(F280-E280)</f>
+        <v>0.14144536852836603</v>
+      </c>
     </row>
     <row r="281" spans="1:16374" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="6">
@@ -58891,6 +58960,10 @@
         <f>AC283/((L283+W283)/2)</f>
         <v>0.19771832070692213</v>
       </c>
+      <c r="AF283" s="24">
+        <f>ABS(F283-E283)</f>
+        <v>0.13778790831565857</v>
+      </c>
     </row>
     <row r="284" spans="1:16374" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="16">
@@ -59159,6 +59232,10 @@
         <f>AC286/((L286+W286)/2)</f>
         <v>0.22600504220946291</v>
       </c>
+      <c r="AF286" s="24">
+        <f>ABS(F286-E286)</f>
+        <v>0.16007953882217407</v>
+      </c>
     </row>
     <row r="287" spans="1:16374" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="6">
@@ -59328,7 +59405,7 @@
         <v>0.235364630818367</v>
       </c>
     </row>
-    <row r="289" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="34">
         <f t="shared" si="4"/>
         <v>96</v>
@@ -59427,8 +59504,12 @@
         <f>AC289/((L289+W289)/2)</f>
         <v>0.62796511140177558</v>
       </c>
+      <c r="AF289" s="24">
+        <f>ABS(F289-E289)</f>
+        <v>0.16637402772903442</v>
+      </c>
     </row>
-    <row r="290" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="16">
         <f t="shared" si="4"/>
         <v>96</v>
@@ -59512,7 +59593,7 @@
         <v>2.306444406509399</v>
       </c>
     </row>
-    <row r="291" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="6">
         <f t="shared" si="4"/>
         <v>97</v>
@@ -59596,7 +59677,7 @@
         <v>0.41754764318466192</v>
       </c>
     </row>
-    <row r="292" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="6">
         <f t="shared" si="4"/>
         <v>97</v>
@@ -59695,8 +59776,12 @@
         <f>AC292/((L292+W292)/2)</f>
         <v>8.6803511031208674E-2</v>
       </c>
+      <c r="AF292" s="24">
+        <f>ABS(F292-E292)</f>
+        <v>0.16532906889915466</v>
+      </c>
     </row>
-    <row r="293" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="6">
         <f t="shared" si="4"/>
         <v>97</v>
@@ -59780,7 +59865,7 @@
         <v>2.2297439575195308</v>
       </c>
     </row>
-    <row r="294" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="10">
         <f t="shared" si="4"/>
         <v>98</v>
@@ -59864,7 +59949,7 @@
         <v>0.35438531637191772</v>
       </c>
     </row>
-    <row r="295" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="13">
         <f t="shared" si="4"/>
         <v>98</v>
@@ -59963,8 +60048,12 @@
         <f>AC295/((L295+W295)/2)</f>
         <v>0.12347308045768803</v>
       </c>
+      <c r="AF295" s="24">
+        <f>ABS(F295-E295)</f>
+        <v>0.13720297813415522</v>
+      </c>
     </row>
-    <row r="296" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="16">
         <f t="shared" si="4"/>
         <v>98</v>
@@ -60048,7 +60137,7 @@
         <v>2.653538703918457</v>
       </c>
     </row>
-    <row r="297" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="6">
         <f t="shared" si="4"/>
         <v>99</v>
@@ -60132,7 +60221,7 @@
         <v>0.43493521213531489</v>
       </c>
     </row>
-    <row r="298" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="6">
         <f t="shared" si="4"/>
         <v>99</v>
@@ -60232,7 +60321,7 @@
         <v>0.51685926479632827</v>
       </c>
     </row>
-    <row r="299" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="6">
         <f t="shared" si="4"/>
         <v>99</v>
@@ -60316,7 +60405,7 @@
         <v>2.401000022888184</v>
       </c>
     </row>
-    <row r="300" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="10">
         <f t="shared" si="4"/>
         <v>100</v>
@@ -60400,7 +60489,7 @@
         <v>0.54546570777893066</v>
       </c>
     </row>
-    <row r="301" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="13">
         <f t="shared" si="4"/>
         <v>100</v>
@@ -60500,7 +60589,7 @@
         <v>0.42753920519470556</v>
       </c>
     </row>
-    <row r="302" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="16">
         <f t="shared" si="4"/>
         <v>100</v>
@@ -60584,7 +60673,7 @@
         <v>2.54743480682373</v>
       </c>
     </row>
-    <row r="303" spans="1:31" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C303" s="8"/>
       <c r="AB303" s="24">
         <f>MAX(AB4:AB301)</f>
@@ -60599,7 +60688,7 @@
         <v>0.11911940574645996</v>
       </c>
     </row>
-    <row r="304" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:32" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C304" s="8"/>
       <c r="AB304" s="24">
         <f>MAX(AB4:AB301)</f>
@@ -60906,7 +60995,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AE303" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A2:AE304" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="y"/>
@@ -60925,69 +61014,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20057EC1-A022-4843-9AA1-49E4543CC77A}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="49"/>
-    <col min="2" max="2" width="201.42578125" style="49" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="49"/>
+    <col min="1" max="1" width="11.42578125" style="45"/>
+    <col min="2" max="2" width="201.42578125" style="45" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="45"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="49">
+      <c r="A1" s="45">
         <v>1</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="45" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="45" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="49">
+      <c r="A4" s="45">
         <v>2</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="45" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="49">
+      <c r="A7" s="45">
         <v>3</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="45" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="45" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="49">
+      <c r="A10" s="45">
         <v>4</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="45" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="49">
+      <c r="A12" s="45">
         <v>5</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="45" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>